<commit_message>
Scoring is now more balanced
</commit_message>
<xml_diff>
--- a/Behaviour Outcomes.xlsx
+++ b/Behaviour Outcomes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2112" windowWidth="19200" windowHeight="8790"/>
+    <workbookView xWindow="0" yWindow="2715" windowWidth="19200" windowHeight="8790"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>State</t>
   </si>
@@ -104,15 +104,36 @@
     <t>Sneak past guard</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>Logic will be</t>
+  </si>
+  <si>
+    <t>&gt; 7 V + &lt;7 S = V</t>
+  </si>
+  <si>
+    <t>&lt;7V + &gt;7S = S</t>
+  </si>
+  <si>
+    <t>&lt;7V + &lt;7S | &gt;7V +&gt;7S = Fail</t>
+  </si>
+  <si>
+    <t>0V + 3S Accidental human easter egg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -140,8 +161,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,7 +660,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D19" totalsRowCount="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D18">
   <autoFilter ref="A1:D18"/>
   <tableColumns count="4">
     <tableColumn id="1" name="State" totalsRowLabel="Total"/>
@@ -913,22 +935,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83984375" customWidth="1"/>
-    <col min="2" max="2" width="19.20703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.26171875" customWidth="1"/>
-    <col min="4" max="4" width="12.15625" customWidth="1"/>
-    <col min="5" max="8" width="8.83984375" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="8" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -942,7 +964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -955,8 +977,11 @@
       <c r="D2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -969,8 +994,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -983,8 +1011,11 @@
       <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -997,8 +1028,11 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1011,8 +1045,11 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1026,7 +1063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1037,10 +1074,10 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1054,7 +1091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1068,7 +1105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1082,7 +1119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1096,7 +1133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1110,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1124,7 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1138,7 +1175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1152,7 +1189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1166,7 +1203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1178,19 +1215,6 @@
       </c>
       <c r="D18">
         <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19">
-        <f>SUBTOTAL(109,Table1[Violent Score])</f>
-        <v>15</v>
-      </c>
-      <c r="D19">
-        <f>SUBTOTAL(109,Table1[Smart Score])</f>
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a violent score for forcing the door to balance scoring
</commit_message>
<xml_diff>
--- a/Behaviour Outcomes.xlsx
+++ b/Behaviour Outcomes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3315" windowWidth="19200" windowHeight="8790"/>
+    <workbookView xWindow="0" yWindow="3915" windowWidth="19200" windowHeight="8790"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t>Shout through door</t>
   </si>
   <si>
-    <t>Push door</t>
-  </si>
-  <si>
     <t>Try handle</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>0V + 3S Accidental human easter egg</t>
+  </si>
+  <si>
+    <t>Force door</t>
   </si>
 </sst>
 </file>
@@ -938,7 +938,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,7 +978,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -995,7 +995,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1012,7 +1012,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1029,7 +1029,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1046,7 +1046,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1110,10 +1110,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1124,7 +1124,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1135,10 +1135,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
         <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1149,10 +1149,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -1163,10 +1163,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1177,10 +1177,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1191,10 +1191,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1205,10 +1205,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>0</v>

</xml_diff>

<commit_message>
Game has passed all outcoem tests successfully after some small in test fixes
</commit_message>
<xml_diff>
--- a/Behaviour Outcomes.xlsx
+++ b/Behaviour Outcomes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3915" windowWidth="19200" windowHeight="8790"/>
+    <workbookView xWindow="0" yWindow="4515" windowWidth="19200" windowHeight="8790"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -938,7 +938,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,7 +1006,7 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1023,10 +1023,10 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="s">
         <v>28</v>
@@ -1057,7 +1057,7 @@
         <v>13</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1071,7 +1071,7 @@
         <v>14</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1085,10 +1085,10 @@
         <v>15</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1113,7 +1113,7 @@
         <v>30</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1130,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1169,7 +1169,7 @@
         <v>21</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1183,7 +1183,7 @@
         <v>22</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16">
         <v>1</v>

</xml_diff>